<commit_message>
Adjusted scripts for fixed point accuracy study. Now runs properly on Cedar
</commit_message>
<xml_diff>
--- a/asic/fixed_point_accuracy_study/results/results_template.xlsx
+++ b/asic/fixed_point_accuracy_study/results/results_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4852EB7F-9890-DE4D-8764-67239B8270E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A5A792-2A61-7F44-9F6E-BE18162B2E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{1EDA0C70-5E08-2840-836D-0713233E97B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Fixed-point accuracy study</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>N_STO = 20</t>
+  </si>
+  <si>
+    <t>N_STO = 7</t>
   </si>
 </sst>
 </file>
@@ -206,12 +209,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A05F66-FDA4-1C44-983C-5A57F89EBD64}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,14 +561,15 @@
     <col min="2" max="2" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -575,42 +580,45 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed-point accuracy study is now fully functional, with adjustable width, dynamic format and a separate format for weights.
</commit_message>
<xml_diff>
--- a/asic/fixed_point_accuracy_study/results/results_template.xlsx
+++ b/asic/fixed_point_accuracy_study/results/results_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trobitaille\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A5A792-2A61-7F44-9F6E-BE18162B2E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D807D2-B50A-4188-8913-AF2F7E067B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{1EDA0C70-5E08-2840-836D-0713233E97B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{1EDA0C70-5E08-2840-836D-0713233E97B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Fixed-point accuracy study</t>
   </si>
@@ -90,13 +90,28 @@
   </si>
   <si>
     <t>N_STO = 7</t>
+  </si>
+  <si>
+    <t>N_STO = 4</t>
+  </si>
+  <si>
+    <t>N_STO = 5</t>
+  </si>
+  <si>
+    <t>N_STO = 6</t>
+  </si>
+  <si>
+    <t>N_STO = 2</t>
+  </si>
+  <si>
+    <t>N_STO = 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -550,26 +565,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A05F66-FDA4-1C44-983C-5A57F89EBD64}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="21">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -580,45 +600,60 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>